<commit_message>
Nombre de estaciones en Coordenadas de estaciones y correción en doc
</commit_message>
<xml_diff>
--- a/Coordenadas_estaciones.xlsx
+++ b/Coordenadas_estaciones.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjuarez\Downloads\DatosSusana\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Compartido\Big Data\Github\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C86D372-9D11-49E5-87AC-6920000B3080}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7740"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
   <si>
     <t>03°22'40,0"W</t>
   </si>
@@ -336,12 +337,159 @@
   </si>
   <si>
     <t>Longitud</t>
+  </si>
+  <si>
+    <t>NOMBRE_ESTACION</t>
+  </si>
+  <si>
+    <t>PLAZA ESPAÑA</t>
+  </si>
+  <si>
+    <t>ESCUELAS AGUIRRE</t>
+  </si>
+  <si>
+    <t>AVDA. RAMÓN Y CAJAL</t>
+  </si>
+  <si>
+    <t>ARTURO SORIA</t>
+  </si>
+  <si>
+    <t>VILLAVERDE</t>
+  </si>
+  <si>
+    <t>FAROLILLO</t>
+  </si>
+  <si>
+    <t>CASA DE CAMPO</t>
+  </si>
+  <si>
+    <t>BARAJAS PUEBLO</t>
+  </si>
+  <si>
+    <t>PLAZA DEL CARMEN</t>
+  </si>
+  <si>
+    <t>MORATALAZ</t>
+  </si>
+  <si>
+    <t>CUATRO CAMINOS</t>
+  </si>
+  <si>
+    <t>BARRIO DEL PILAR</t>
+  </si>
+  <si>
+    <t>VALLECAS</t>
+  </si>
+  <si>
+    <t>MENDEZ ÁLVARO</t>
+  </si>
+  <si>
+    <t>CASTELLANA</t>
+  </si>
+  <si>
+    <t>PARQUE DEL RETIRO</t>
+  </si>
+  <si>
+    <t>PLAZA CASTILLA</t>
+  </si>
+  <si>
+    <t>ENSANCHE DE VALLECAS</t>
+  </si>
+  <si>
+    <t>URB. EMBAJADA</t>
+  </si>
+  <si>
+    <t>PLAZA ELÍPTICA</t>
+  </si>
+  <si>
+    <t>SANCHINARRO</t>
+  </si>
+  <si>
+    <t>EL PARDO</t>
+  </si>
+  <si>
+    <t>JUAN CARLOS I</t>
+  </si>
+  <si>
+    <t>TRES OLIVOS</t>
+  </si>
+  <si>
+    <t>ALCALÁ DE HENARES</t>
+  </si>
+  <si>
+    <t>ALCOBENDAS</t>
+  </si>
+  <si>
+    <t>ALCORCÓN</t>
+  </si>
+  <si>
+    <t>ALGETE</t>
+  </si>
+  <si>
+    <t>ARANJUEZ</t>
+  </si>
+  <si>
+    <t>ARGANDA DEL REY</t>
+  </si>
+  <si>
+    <t>EL ATAZAR</t>
+  </si>
+  <si>
+    <t>COLMENAR VIEJO</t>
+  </si>
+  <si>
+    <t>COLLADO VILLALBA</t>
+  </si>
+  <si>
+    <t>COSLADA</t>
+  </si>
+  <si>
+    <t>FUENLABRADA</t>
+  </si>
+  <si>
+    <t>GETAFE</t>
+  </si>
+  <si>
+    <t>GUADALIX DE LA SIERRA</t>
+  </si>
+  <si>
+    <t>LEGANÉS</t>
+  </si>
+  <si>
+    <t>MAJADAHONDA</t>
+  </si>
+  <si>
+    <t>MÓSTOLES</t>
+  </si>
+  <si>
+    <t>ORUSCO DE TAJUÑA</t>
+  </si>
+  <si>
+    <t>PUERTO DE COTOS</t>
+  </si>
+  <si>
+    <t>RIVAS-VACIAMADRID</t>
+  </si>
+  <si>
+    <t>SAN MARTÍN DE VALDEIGLESIAS</t>
+  </si>
+  <si>
+    <t>TORREJÓN DE ARDOZ</t>
+  </si>
+  <si>
+    <t>VALDEMORO</t>
+  </si>
+  <si>
+    <t>VILLA DEL PRADO</t>
+  </si>
+  <si>
+    <t>VILLAREJO DE SALVANÉS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -858,7 +1006,7 @@
     <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
@@ -972,6 +1120,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1007,6 +1172,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1182,11 +1364,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,1285 +1377,1431 @@
     <col min="2" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="7">
         <v>28079004</v>
       </c>
-      <c r="B2" s="7">
+      <c r="C2" s="7">
         <v>439579.32909999997</v>
       </c>
-      <c r="C2" s="7">
+      <c r="D2" s="5">
         <v>4475049.2630000003</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="9">
+      <c r="G2" s="9">
         <v>-37122567</v>
       </c>
-      <c r="G2" s="9">
+      <c r="H2" s="9">
         <v>404238823</v>
       </c>
-      <c r="H2">
-        <v>-3.7121972222222199</v>
-      </c>
       <c r="I2">
-        <v>40.423883333333301</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+        <v>-3.7121972219999999</v>
+      </c>
+      <c r="J2">
+        <v>40.423883330000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="7">
         <v>28079008</v>
       </c>
-      <c r="B3" s="7">
+      <c r="C3" s="7">
         <v>442117.2366</v>
       </c>
-      <c r="C3" s="7">
+      <c r="D3" s="5">
         <v>4474770.6960000005</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="9">
+      <c r="G3" s="9">
         <v>-36823158</v>
       </c>
-      <c r="G3" s="9">
+      <c r="H3" s="9">
         <v>404215533</v>
       </c>
-      <c r="H3">
-        <v>-3.6822833333333298</v>
-      </c>
       <c r="I3">
-        <v>40.421563888888798</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+        <v>-3.682283333</v>
+      </c>
+      <c r="J3">
+        <v>40.421563890000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="7">
         <v>28079011</v>
       </c>
-      <c r="B4" s="7">
+      <c r="C4" s="7">
         <v>442564.04570000002</v>
       </c>
-      <c r="C4" s="7">
+      <c r="D4" s="5">
         <v>4478088.5949999997</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="9">
+      <c r="G4" s="9">
         <v>-36773491</v>
       </c>
-      <c r="G4" s="9">
+      <c r="H4" s="9">
         <v>404514734</v>
       </c>
-      <c r="H4">
-        <v>-3.67736111111111</v>
-      </c>
       <c r="I4">
-        <v>40.451469444444399</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+        <v>-3.6773611110000002</v>
+      </c>
+      <c r="J4">
+        <v>40.451469439999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="7">
         <v>28079016</v>
       </c>
-      <c r="B5" s="7">
+      <c r="C5" s="7">
         <v>445786.17290000001</v>
       </c>
-      <c r="C5" s="7">
+      <c r="D5" s="5">
         <v>4476796.0190000003</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="9">
+      <c r="G5" s="9">
         <v>-36392422</v>
       </c>
-      <c r="G5" s="9">
+      <c r="H5" s="9">
         <v>404400457</v>
       </c>
-      <c r="H5">
-        <v>-3.6392138888888801</v>
-      </c>
       <c r="I5">
-        <v>40.440055555555503</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+        <v>-3.6392138890000001</v>
+      </c>
+      <c r="J5">
+        <v>40.440055559999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="7">
         <v>28079017</v>
       </c>
-      <c r="B6" s="7">
+      <c r="C6" s="7">
         <v>439420.70150000002</v>
       </c>
-      <c r="C6" s="7">
+      <c r="D6" s="5">
         <v>4466532.4550000001</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="9">
+      <c r="G6" s="9">
         <v>-37133167</v>
       </c>
-      <c r="G6" s="9">
+      <c r="H6" s="9">
         <v>40347147</v>
       </c>
-      <c r="H6">
-        <v>-3.7133027777777698</v>
-      </c>
       <c r="I6">
+        <v>-3.7133027780000001</v>
+      </c>
+      <c r="J6">
         <v>40.347149999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="7">
         <v>28079018</v>
       </c>
-      <c r="B7" s="7">
+      <c r="C7" s="7">
         <v>437891.6961</v>
       </c>
-      <c r="C7" s="7">
+      <c r="D7" s="5">
         <v>4471832.7690000003</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="9">
+      <c r="G7" s="9">
         <v>-37318356</v>
       </c>
-      <c r="G7" s="9">
+      <c r="H7" s="9">
         <v>403947825</v>
       </c>
-      <c r="H7">
-        <v>-3.73183611111111</v>
-      </c>
       <c r="I7">
-        <v>40.394783333333301</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+        <v>-3.7318361109999998</v>
+      </c>
+      <c r="J7">
+        <v>40.394783330000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="7">
         <v>28079024</v>
       </c>
-      <c r="B8" s="7">
+      <c r="C8" s="7">
         <v>436598.5637</v>
       </c>
-      <c r="C8" s="7">
+      <c r="D8" s="5">
         <v>4474571.6179999998</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F8" s="9">
+      <c r="G8" s="9">
         <v>-37473445</v>
       </c>
-      <c r="G8" s="9">
+      <c r="H8" s="9">
         <v>404193577</v>
       </c>
-      <c r="H8">
-        <v>-3.7473444444444399</v>
-      </c>
       <c r="I8">
-        <v>40.4193583333333</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+        <v>-3.7473444439999999</v>
+      </c>
+      <c r="J8">
+        <v>40.419358330000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="7">
         <v>28079027</v>
       </c>
-      <c r="B9" s="7">
+      <c r="C9" s="7">
         <v>450835.20260000002</v>
       </c>
-      <c r="C9" s="7">
+      <c r="D9" s="5">
         <v>4480854.1720000003</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="9">
+      <c r="G9" s="9">
         <v>-35800258</v>
       </c>
-      <c r="G9" s="9">
+      <c r="H9" s="9">
         <v>404769179</v>
       </c>
-      <c r="H9">
-        <v>-3.58002777777777</v>
-      </c>
       <c r="I9">
+        <v>-3.5800277779999998</v>
+      </c>
+      <c r="J9">
         <v>40.476925000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="7">
         <v>28079035</v>
       </c>
-      <c r="B10" s="7">
+      <c r="C10" s="7">
         <v>440346.36190000002</v>
       </c>
-      <c r="C10" s="7">
+      <c r="D10" s="5">
         <v>4474524.3569999998</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="9">
+      <c r="G10" s="9">
         <v>-37031662</v>
       </c>
-      <c r="G10" s="9">
+      <c r="H10" s="9">
         <v>404192091</v>
       </c>
-      <c r="H10">
-        <v>-3.7031666666666601</v>
-      </c>
       <c r="I10">
-        <v>40.419208333333302</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+        <v>-3.7031666670000001</v>
+      </c>
+      <c r="J10">
+        <v>40.419208329999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="7">
         <v>28079036</v>
       </c>
-      <c r="B11" s="7">
+      <c r="C11" s="7">
         <v>445245.51299999998</v>
       </c>
-      <c r="C11" s="7">
+      <c r="D11" s="5">
         <v>4473237.3490000004</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="9">
+      <c r="G11" s="9">
         <v>-36453104</v>
       </c>
-      <c r="G11" s="9">
+      <c r="H11" s="9">
         <v>404079517</v>
       </c>
-      <c r="H11">
-        <v>-3.6452833333333299</v>
-      </c>
       <c r="I11">
-        <v>40.407955555555503</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+        <v>-3.6452833330000001</v>
+      </c>
+      <c r="J11">
+        <v>40.407955559999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="7">
         <v>28079038</v>
       </c>
-      <c r="B12" s="7">
+      <c r="C12" s="7">
         <v>440033.4632</v>
       </c>
-      <c r="C12" s="7">
+      <c r="D12" s="5">
         <v>4477450.2110000001</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="9">
+      <c r="G12" s="9">
         <v>-37071303</v>
       </c>
-      <c r="G12" s="9">
+      <c r="H12" s="9">
         <v>404455439</v>
       </c>
-      <c r="H12">
-        <v>-3.7071222222222202</v>
-      </c>
       <c r="I12">
-        <v>40.445547222222203</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+        <v>-3.7071222220000002</v>
+      </c>
+      <c r="J12">
+        <v>40.445547220000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="7">
         <v>28079039</v>
       </c>
-      <c r="B13" s="7">
+      <c r="C13" s="7">
         <v>439689.04960000003</v>
       </c>
-      <c r="C13" s="7">
+      <c r="D13" s="5">
         <v>4481081.6189999999</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="9">
+      <c r="G13" s="9">
         <v>-37115364</v>
       </c>
-      <c r="G13" s="9">
+      <c r="H13" s="9">
         <v>404782322</v>
       </c>
-      <c r="H13">
-        <v>-3.7115361111111098</v>
-      </c>
       <c r="I13">
-        <v>40.4782333333333</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+        <v>-3.711536111</v>
+      </c>
+      <c r="J13">
+        <v>40.478233330000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="7">
         <v>28079040</v>
       </c>
-      <c r="B14" s="7">
+      <c r="C14" s="7">
         <v>444701.68709999998</v>
       </c>
-      <c r="C14" s="7">
+      <c r="D14" s="5">
         <v>4471043.01</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="9">
+      <c r="G14" s="9">
         <v>-36515286</v>
       </c>
-      <c r="G14" s="9">
+      <c r="H14" s="9">
         <v>403881478</v>
       </c>
-      <c r="H14">
-        <v>-3.6515277777777699</v>
-      </c>
       <c r="I14">
-        <v>40.388147222222202</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+        <v>-3.6515277780000002</v>
+      </c>
+      <c r="J14">
+        <v>40.38814722</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="7">
         <v>28079047</v>
       </c>
-      <c r="B15" s="7">
+      <c r="C15" s="7">
         <v>441715.43030000001</v>
       </c>
-      <c r="C15" s="7">
+      <c r="D15" s="5">
         <v>4472170.2489999998</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="9">
+      <c r="G15" s="9">
         <v>-36868138</v>
       </c>
-      <c r="G15" s="9">
+      <c r="H15" s="9">
         <v>403980991</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>-3.6868249999999998</v>
       </c>
-      <c r="I15">
-        <v>40.398102777777702</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="J15">
+        <v>40.398102780000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="7">
         <v>28079048</v>
       </c>
-      <c r="B16" s="7">
+      <c r="C16" s="7">
         <v>441449.63410000002</v>
       </c>
-      <c r="C16" s="7">
+      <c r="D16" s="5">
         <v>4476811.42</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="F16" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F16" s="9">
+      <c r="G16" s="9">
         <v>-36903729</v>
       </c>
-      <c r="G16" s="9">
+      <c r="H16" s="9">
         <v>404398904</v>
       </c>
-      <c r="H16">
-        <v>-3.6903722222222202</v>
-      </c>
       <c r="I16">
-        <v>40.439891666666597</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+        <v>-3.6903722220000001</v>
+      </c>
+      <c r="J16">
+        <v>40.439891670000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="7">
         <v>28079049</v>
       </c>
-      <c r="B17" s="7">
+      <c r="C17" s="7">
         <v>442095.52</v>
       </c>
-      <c r="C17" s="7">
+      <c r="D17" s="5">
         <v>4473981.74</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F17" s="9">
+      <c r="G17" s="9">
         <v>-3.6824999999999904E+16</v>
       </c>
-      <c r="G17" s="9">
+      <c r="H17" s="9">
         <v>4041444444444440</v>
       </c>
-      <c r="H17">
-        <v>-3.6824999999999899</v>
-      </c>
       <c r="I17">
-        <v>40.414444444444399</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+        <v>-3.6825000000000001</v>
+      </c>
+      <c r="J17">
+        <v>40.414444439999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="7">
         <v>28079050</v>
       </c>
-      <c r="B18" s="7">
+      <c r="C18" s="7">
         <v>441609.9474</v>
       </c>
-      <c r="C18" s="7">
+      <c r="D18" s="5">
         <v>4479662.3459999999</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="9">
+      <c r="G18" s="9">
         <v>-36887449</v>
       </c>
-      <c r="G18" s="9">
+      <c r="H18" s="9">
         <v>404655841</v>
       </c>
-      <c r="H18">
-        <v>-3.6887444444444402</v>
-      </c>
       <c r="I18">
-        <v>40.465583333333299</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+        <v>-3.6887444440000001</v>
+      </c>
+      <c r="J18">
+        <v>40.465583330000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="7">
         <v>28079054</v>
       </c>
-      <c r="B19" s="7">
+      <c r="C19" s="7">
         <v>448033.22629999998</v>
       </c>
-      <c r="C19" s="7">
+      <c r="D19" s="5">
         <v>4469339.0439999998</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="F19" s="9">
+      <c r="G19" s="9">
         <v>-36121394</v>
       </c>
-      <c r="G19" s="9">
+      <c r="H19" s="9">
         <v>403730118</v>
       </c>
-      <c r="H19">
-        <v>-3.6121388888888801</v>
-      </c>
       <c r="I19">
-        <v>40.373011111111097</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+        <v>-3.6121388890000001</v>
+      </c>
+      <c r="J19">
+        <v>40.37301111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="7">
         <v>28079055</v>
       </c>
-      <c r="B20" s="7">
+      <c r="C20" s="7">
         <v>450778.88390000002</v>
       </c>
-      <c r="C20" s="7">
+      <c r="D20" s="5">
         <v>4479238.8629999999</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="F20" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="9">
+      <c r="G20" s="9">
         <v>-35805649</v>
       </c>
-      <c r="G20" s="9">
+      <c r="H20" s="9">
         <v>404623628</v>
       </c>
-      <c r="H20">
-        <v>-3.58056388888888</v>
-      </c>
       <c r="I20">
-        <v>40.462363888888802</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+        <v>-3.580563889</v>
+      </c>
+      <c r="J20">
+        <v>40.462363889999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="7">
         <v>28079056</v>
       </c>
-      <c r="B21" s="7">
+      <c r="C21" s="7">
         <v>438991.91609999997</v>
       </c>
-      <c r="C21" s="7">
+      <c r="D21" s="5">
         <v>4470741.5480000004</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="F21" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F21" s="9">
+      <c r="G21" s="9">
         <v>-37187679</v>
       </c>
-      <c r="G21" s="9">
+      <c r="H21" s="9">
         <v>403850336</v>
       </c>
-      <c r="H21">
-        <v>-3.7187611111111099</v>
-      </c>
       <c r="I21">
-        <v>40.385027777777701</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+        <v>-3.7187611110000001</v>
+      </c>
+      <c r="J21">
+        <v>40.385027780000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="7">
         <v>28079057</v>
       </c>
-      <c r="B22" s="7">
+      <c r="C22" s="7">
         <v>444026.80800000002</v>
       </c>
-      <c r="C22" s="7">
+      <c r="D22" s="5">
         <v>4482820.5810000002</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="F22" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="9">
+      <c r="G22" s="9">
         <v>-36605173</v>
       </c>
-      <c r="G22" s="9">
+      <c r="H22" s="9">
         <v>404942012</v>
       </c>
-      <c r="H22">
-        <v>-3.66051666666666</v>
-      </c>
       <c r="I22">
+        <v>-3.660516667</v>
+      </c>
+      <c r="J22">
         <v>40.494199999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" s="7">
         <v>28079058</v>
       </c>
-      <c r="B23" s="7">
+      <c r="C23" s="7">
         <v>434381.6</v>
       </c>
-      <c r="C23" s="7">
+      <c r="D23" s="5">
         <v>4485548.7</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F23" s="9">
+      <c r="G23" s="9">
         <v>-37746101</v>
       </c>
-      <c r="G23" s="9">
+      <c r="H23" s="9">
         <v>405180701</v>
       </c>
-      <c r="H23">
-        <v>-3.7746166666666601</v>
-      </c>
       <c r="I23">
-        <v>40.518047222222201</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+        <v>-3.7746166670000001</v>
+      </c>
+      <c r="J23">
+        <v>40.51804722</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" s="7">
         <v>28079059</v>
       </c>
-      <c r="B24" s="7">
+      <c r="C24" s="7">
         <v>447744.46659999999</v>
       </c>
-      <c r="C24" s="7">
+      <c r="D24" s="5">
         <v>4479077.6780000003</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="F24" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F24" s="9">
+      <c r="G24" s="9">
         <v>-36163407</v>
       </c>
-      <c r="G24" s="9">
+      <c r="H24" s="9">
         <v>404607255</v>
       </c>
-      <c r="H24">
-        <v>-3.6091666666666602</v>
-      </c>
       <c r="I24">
-        <v>40.4652777777777</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+        <v>-3.6091666670000002</v>
+      </c>
+      <c r="J24">
+        <v>40.465277780000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25" s="7">
         <v>28079060</v>
       </c>
-      <c r="B25" s="7">
+      <c r="C25" s="7">
         <v>441556.70049999998</v>
       </c>
-      <c r="C25" s="7">
+      <c r="D25" s="5">
         <v>4483543.9939999999</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="F25" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="F25" s="9">
+      <c r="G25" s="9">
         <v>-36897308</v>
       </c>
-      <c r="G25" s="9">
+      <c r="H25" s="9">
         <v>405005477</v>
       </c>
-      <c r="H25">
-        <v>-3.68973055555555</v>
-      </c>
       <c r="I25">
-        <v>40.500547222222202</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+        <v>-3.6897305560000002</v>
+      </c>
+      <c r="J25">
+        <v>40.500547220000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" s="2">
         <v>28005002</v>
       </c>
-      <c r="B26" s="2">
+      <c r="C26" s="2">
         <v>467979</v>
       </c>
-      <c r="C26" s="2">
+      <c r="D26" s="2">
         <v>4481011</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" t="s">
         <v>1</v>
       </c>
-      <c r="H26">
-        <v>-3.3777777777777702</v>
-      </c>
       <c r="I26">
-        <v>40.4791666666666</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+        <v>-3.377777778</v>
+      </c>
+      <c r="J26">
+        <v>40.479166669999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" s="2">
         <v>28006004</v>
       </c>
-      <c r="B27" s="2">
+      <c r="C27" s="2">
         <v>445363</v>
       </c>
-      <c r="C27" s="2">
+      <c r="D27" s="2">
         <v>4487950</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" t="s">
         <v>3</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>-3.645</v>
       </c>
-      <c r="I27">
-        <v>40.540277777777703</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="J27">
+        <v>40.540277779999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" s="2">
         <v>28007004</v>
       </c>
-      <c r="B28" s="2">
+      <c r="C28" s="2">
         <v>429190</v>
       </c>
-      <c r="C28" s="2">
+      <c r="D28" s="2">
         <v>4466041</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" t="s">
         <v>5</v>
       </c>
-      <c r="H28">
-        <v>-3.83361111111111</v>
-      </c>
       <c r="I28">
-        <v>40.341666666666598</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+        <v>-3.8336111110000002</v>
+      </c>
+      <c r="J28">
+        <v>40.341666670000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" s="2">
         <v>28009001</v>
       </c>
-      <c r="B29" s="2">
+      <c r="C29" s="2">
         <v>457418</v>
       </c>
-      <c r="C29" s="2">
+      <c r="D29" s="2">
         <v>4494449</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" t="s">
         <v>7</v>
       </c>
-      <c r="H29">
-        <v>-3.5030555555555498</v>
-      </c>
       <c r="I29">
-        <v>40.599722222222198</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+        <v>-3.5030555560000001</v>
+      </c>
+      <c r="J29">
+        <v>40.599722219999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30" s="2">
         <v>28013002</v>
       </c>
-      <c r="B30" s="2">
+      <c r="C30" s="2">
         <v>449541</v>
       </c>
-      <c r="C30" s="2">
+      <c r="D30" s="2">
         <v>4431618</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" t="s">
         <v>9</v>
       </c>
-      <c r="H30">
-        <v>-3.5913888888888801</v>
-      </c>
       <c r="I30">
-        <v>40.033055555555499</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+        <v>-3.5913888890000001</v>
+      </c>
+      <c r="J30">
+        <v>40.033055560000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31" s="2">
         <v>28014002</v>
       </c>
-      <c r="B31" s="2">
+      <c r="C31" s="2">
         <v>461002</v>
       </c>
-      <c r="C31" s="2">
+      <c r="D31" s="2">
         <v>4461246</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" t="s">
         <v>11</v>
       </c>
-      <c r="H31">
-        <v>-3.4588888888888798</v>
-      </c>
       <c r="I31">
-        <v>40.300555555555498</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+        <v>-3.4588888889999998</v>
+      </c>
+      <c r="J31">
+        <v>40.300555559999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32" s="2">
         <v>28016001</v>
       </c>
-      <c r="B32" s="2">
+      <c r="C32" s="2">
         <v>460596</v>
       </c>
-      <c r="C32" s="2">
+      <c r="D32" s="2">
         <v>4528767</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" t="s">
         <v>13</v>
       </c>
-      <c r="H32">
-        <v>-3.4677777777777701</v>
-      </c>
       <c r="I32">
-        <v>40.908888888888796</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+        <v>-3.4677777779999999</v>
+      </c>
+      <c r="J32">
+        <v>40.90888889</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33" s="2">
         <v>28045002</v>
       </c>
-      <c r="B33" s="2">
+      <c r="C33" s="2">
         <v>434586</v>
       </c>
-      <c r="C33" s="2">
+      <c r="D33" s="2">
         <v>4501818</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" t="s">
         <v>15</v>
       </c>
-      <c r="H33">
-        <v>-3.7738888888888802</v>
-      </c>
       <c r="I33">
-        <v>40.664444444444399</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+        <v>-3.7738888890000002</v>
+      </c>
+      <c r="J33">
+        <v>40.664444439999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B34" s="2">
         <v>28047002</v>
       </c>
-      <c r="B34" s="2">
+      <c r="C34" s="2">
         <v>414233</v>
       </c>
-      <c r="C34" s="2">
+      <c r="D34" s="2">
         <v>4498525</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" t="s">
         <v>17</v>
       </c>
-      <c r="H34">
-        <v>-4.01416666666666</v>
-      </c>
       <c r="I34">
-        <v>40.633055555555501</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+        <v>-4.0141666669999996</v>
+      </c>
+      <c r="J34">
+        <v>40.633055560000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="2">
         <v>28049003</v>
       </c>
-      <c r="B35" s="2">
+      <c r="C35" s="2">
         <v>454001</v>
       </c>
-      <c r="C35" s="2">
+      <c r="D35" s="2">
         <v>4475678</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" t="s">
         <v>19</v>
       </c>
-      <c r="H35">
-        <v>-3.5422222222222199</v>
-      </c>
       <c r="I35">
-        <v>40.430277777777697</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+        <v>-3.5422222219999999</v>
+      </c>
+      <c r="J35">
+        <v>40.430277779999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="2">
         <v>28058004</v>
       </c>
-      <c r="B36" s="2">
+      <c r="C36" s="2">
         <v>431913</v>
       </c>
-      <c r="C36" s="2">
+      <c r="D36" s="2">
         <v>4459313</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" t="s">
         <v>21</v>
       </c>
-      <c r="H36">
-        <v>-3.8008333333333302</v>
-      </c>
       <c r="I36">
-        <v>40.281388888888799</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+        <v>-3.8008333329999999</v>
+      </c>
+      <c r="J36">
+        <v>40.281388890000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="2">
         <v>28065014</v>
       </c>
-      <c r="B37" s="2">
+      <c r="C37" s="2">
         <v>439090</v>
       </c>
-      <c r="C37" s="2">
+      <c r="D37" s="2">
         <v>4462920</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="F37" t="s">
         <v>23</v>
       </c>
-      <c r="H37">
-        <v>-3.7166666666666601</v>
-      </c>
       <c r="I37">
-        <v>40.314444444444398</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+        <v>-3.7166666670000001</v>
+      </c>
+      <c r="J37">
+        <v>40.314444440000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38" s="2">
         <v>28067001</v>
       </c>
-      <c r="B38" s="2">
+      <c r="C38" s="2">
         <v>440751</v>
       </c>
-      <c r="C38" s="2">
+      <c r="D38" s="2">
         <v>4514644</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="F38" t="s">
         <v>25</v>
       </c>
-      <c r="H38">
-        <v>-3.70194444444444</v>
-      </c>
       <c r="I38">
-        <v>40.780555555555502</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+        <v>-3.701944444</v>
+      </c>
+      <c r="J38">
+        <v>40.780555560000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39" s="2">
         <v>28074007</v>
       </c>
-      <c r="B39" s="2">
+      <c r="C39" s="2">
         <v>435914</v>
       </c>
-      <c r="C39" s="2">
+      <c r="D39" s="2">
         <v>4465744</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="F39" t="s">
         <v>27</v>
       </c>
-      <c r="H39">
-        <v>-3.7544444444444398</v>
-      </c>
       <c r="I39">
-        <v>40.3397222222222</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+        <v>-3.7544444440000002</v>
+      </c>
+      <c r="J39">
+        <v>40.339722219999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B40" s="2">
         <v>28080003</v>
       </c>
-      <c r="B40" s="2">
+      <c r="C40" s="2">
         <v>426307</v>
       </c>
-      <c r="C40" s="2">
+      <c r="D40" s="2">
         <v>4477645</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="F40" t="s">
         <v>29</v>
       </c>
-      <c r="H40">
-        <v>-3.8688888888888799</v>
-      </c>
       <c r="I40">
-        <v>40.446111111111101</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+        <v>-3.8688888889999999</v>
+      </c>
+      <c r="J40">
+        <v>40.446111109999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B41" s="2">
         <v>28092005</v>
       </c>
-      <c r="B41" s="2">
+      <c r="C41" s="2">
         <v>425516</v>
       </c>
-      <c r="C41" s="2">
+      <c r="D41" s="2">
         <v>4464113</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="F41" t="s">
         <v>31</v>
       </c>
-      <c r="H41">
-        <v>-3.8766666666666598</v>
-      </c>
       <c r="I41">
-        <v>40.324166666666599</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+        <v>-3.8766666669999998</v>
+      </c>
+      <c r="J41">
+        <v>40.324166669999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" s="2">
         <v>28102001</v>
       </c>
-      <c r="B42" s="2">
+      <c r="C42" s="2">
         <v>481205</v>
       </c>
-      <c r="C42" s="2">
+      <c r="D42" s="2">
         <v>4459700</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="F42" t="s">
         <v>33</v>
       </c>
-      <c r="H42">
-        <v>-3.2211111111111101</v>
-      </c>
       <c r="I42">
+        <v>-3.2211111109999999</v>
+      </c>
+      <c r="J42">
         <v>40.287500000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B43" s="2">
         <v>28120001</v>
       </c>
-      <c r="B43" s="2">
+      <c r="C43" s="2">
         <v>418948</v>
       </c>
-      <c r="C43" s="2">
+      <c r="D43" s="2">
         <v>4519788</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="F43" t="s">
         <v>35</v>
       </c>
-      <c r="H43">
-        <v>-3.9611111111111099</v>
-      </c>
       <c r="I43">
+        <v>-3.9611111110000001</v>
+      </c>
+      <c r="J43">
         <v>40.825000000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B44" s="2">
         <v>28123002</v>
       </c>
-      <c r="B44" s="2">
+      <c r="C44" s="2">
         <v>453906</v>
       </c>
-      <c r="C44" s="2">
+      <c r="D44" s="2">
         <v>4467829</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="F44" t="s">
         <v>37</v>
       </c>
-      <c r="H44">
-        <v>-3.5427777777777698</v>
-      </c>
       <c r="I44">
-        <v>40.359722222222203</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+        <v>-3.542777778</v>
+      </c>
+      <c r="J44">
+        <v>40.359722220000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B45" s="2">
         <v>28133002</v>
       </c>
-      <c r="B45" s="2">
+      <c r="C45" s="2">
         <v>381298</v>
       </c>
-      <c r="C45" s="2">
+      <c r="D45" s="2">
         <v>4469513</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="F45" t="s">
         <v>39</v>
       </c>
-      <c r="H45">
-        <v>-4.3980555555555503</v>
-      </c>
       <c r="I45">
+        <v>-4.3980555560000001</v>
+      </c>
+      <c r="J45">
         <v>40.3675</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B46" s="2">
         <v>28148004</v>
       </c>
-      <c r="B46" s="2">
+      <c r="C46" s="2">
         <v>459497</v>
       </c>
-      <c r="C46" s="2">
+      <c r="D46" s="2">
         <v>4477765</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="F46" t="s">
         <v>41</v>
       </c>
-      <c r="H46">
+      <c r="I46">
         <v>-3.4775</v>
       </c>
-      <c r="I46">
-        <v>40.449444444444403</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
+      <c r="J46">
+        <v>40.449444440000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B47" s="2">
         <v>28161001</v>
       </c>
-      <c r="B47" s="2">
+      <c r="C47" s="2">
         <v>442089</v>
       </c>
-      <c r="C47" s="2">
+      <c r="D47" s="2">
         <v>4448540</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="F47" t="s">
         <v>43</v>
       </c>
-      <c r="H47">
-        <v>-3.68027777777777</v>
-      </c>
       <c r="I47">
-        <v>40.184999999999903</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+        <v>-3.6802777780000002</v>
+      </c>
+      <c r="J47">
+        <v>40.185000000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B48" s="2">
         <v>28171001</v>
       </c>
-      <c r="B48" s="2">
+      <c r="C48" s="2">
         <v>391504</v>
       </c>
-      <c r="C48" s="2">
+      <c r="D48" s="2">
         <v>4456144</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="F48" t="s">
         <v>45</v>
       </c>
-      <c r="H48">
-        <v>-4.2755555555555498</v>
-      </c>
       <c r="I48">
-        <v>40.248611111111103</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+        <v>-4.2755555559999996</v>
+      </c>
+      <c r="J48">
+        <v>40.248611109999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B49" s="2">
         <v>28180001</v>
       </c>
-      <c r="B49" s="2">
+      <c r="C49" s="2">
         <v>476442</v>
       </c>
-      <c r="C49" s="2">
+      <c r="D49" s="2">
         <v>4446354</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="F49" t="s">
         <v>47</v>
       </c>
-      <c r="H49">
-        <v>-3.2766666666666602</v>
-      </c>
       <c r="I49">
-        <v>40.1672222222222</v>
+        <v>-3.2766666670000002</v>
+      </c>
+      <c r="J49">
+        <v>40.167222219999999</v>
       </c>
     </row>
   </sheetData>
@@ -2482,7 +2810,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2494,7 +2822,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Coordenadas estaciones con la dirección y nombre
Coordenadas estaciones con la dirección y nombre.
</commit_message>
<xml_diff>
--- a/Coordenadas_estaciones.xlsx
+++ b/Coordenadas_estaciones.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjuarez\Downloads\DatosSusana\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7740"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="211">
   <si>
     <t>03°22'40,0"W</t>
   </si>
@@ -320,12 +315,6 @@
     <t>COORDENADA_Y_ETRS89</t>
   </si>
   <si>
-    <t>LONGITUD</t>
-  </si>
-  <si>
-    <t>LATITUD</t>
-  </si>
-  <si>
     <t>3°40' 57''O</t>
   </si>
   <si>
@@ -336,6 +325,330 @@
   </si>
   <si>
     <t>Longitud</t>
+  </si>
+  <si>
+    <t>ESTACION</t>
+  </si>
+  <si>
+    <t>DIRECCION</t>
+  </si>
+  <si>
+    <t>Pza. de España</t>
+  </si>
+  <si>
+    <t>Plaza de España</t>
+  </si>
+  <si>
+    <t>Escuelas Aguirre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entre C/ Alcalá y C/ O’ Donell </t>
+  </si>
+  <si>
+    <t>Avda. Ramón y Cajal</t>
+  </si>
+  <si>
+    <t>Avda. Ramón y Cajal  esq. C/ Príncipe de Vergara</t>
+  </si>
+  <si>
+    <t>Arturo Soria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C/ Arturo Soria  esq. C/  Vizconde de los Asilos </t>
+  </si>
+  <si>
+    <t>Villaverde</t>
+  </si>
+  <si>
+    <t>C/. Juan Peñalver</t>
+  </si>
+  <si>
+    <t>Farolillo</t>
+  </si>
+  <si>
+    <t>Calle Farolillo - C/Ervigio</t>
+  </si>
+  <si>
+    <t>Casa de Campo</t>
+  </si>
+  <si>
+    <t>Casa de Campo  (Terminal del Teleférico)</t>
+  </si>
+  <si>
+    <t>Barajas Pueblo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C/. Júpiter, 21 (Barajas) </t>
+  </si>
+  <si>
+    <t>Pza. del Carmen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plaza del Carmen esq. Tres Cruces. </t>
+  </si>
+  <si>
+    <t>Moratalaz</t>
+  </si>
+  <si>
+    <t>Avd. Moratalaz  esq. Camino de los Vinateros</t>
+  </si>
+  <si>
+    <t>Cuatro Caminos</t>
+  </si>
+  <si>
+    <t>Avda. Pablo Iglesias esq. C/ Marqués de Lema</t>
+  </si>
+  <si>
+    <t>Barrio del Pilar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avd. Betanzos esq. C/  Monforte de Lemos </t>
+  </si>
+  <si>
+    <t>Vallecas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C/ Arroyo del Olivar  esq. C/  Río Grande. </t>
+  </si>
+  <si>
+    <t>Mendez Alvaro</t>
+  </si>
+  <si>
+    <t>C/ Juan de Mariana / Pza. Amanecer Mendez Alvaro</t>
+  </si>
+  <si>
+    <t>Castellana</t>
+  </si>
+  <si>
+    <t>C/ Jose Gutierrez Abascal</t>
+  </si>
+  <si>
+    <t>Parque del Retiro</t>
+  </si>
+  <si>
+    <t>Paseo Venezuela- Casa de Vacas</t>
+  </si>
+  <si>
+    <t>Plaza Castilla</t>
+  </si>
+  <si>
+    <t>Plaza Castilla (Canal)</t>
+  </si>
+  <si>
+    <t>Ensanche de Vallecas</t>
+  </si>
+  <si>
+    <t>Avda La Gavia / Avda. Las Suertes</t>
+  </si>
+  <si>
+    <t>Urb. Embajada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C/ Riaño (Barajas) </t>
+  </si>
+  <si>
+    <t>Pza. Elíptica</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pza. Elíptica - Avda. Oporto</t>
+  </si>
+  <si>
+    <t>Sanchinarro</t>
+  </si>
+  <si>
+    <t>C/ Princesa de Eboli esq C/ Maria Tudor</t>
+  </si>
+  <si>
+    <t>El Pardo</t>
+  </si>
+  <si>
+    <t>Avda. La Guardia</t>
+  </si>
+  <si>
+    <t>Juan Carlos I</t>
+  </si>
+  <si>
+    <t>Parque Juan Carlos I (frente oficinas mantenimiento)</t>
+  </si>
+  <si>
+    <t>Tres Olivos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plaza Tres Olivos </t>
+  </si>
+  <si>
+    <t>Alcalá de Henares</t>
+  </si>
+  <si>
+    <t>Alcobendas</t>
+  </si>
+  <si>
+    <t>Alcorcón</t>
+  </si>
+  <si>
+    <t>Algete</t>
+  </si>
+  <si>
+    <t>Aranjuez</t>
+  </si>
+  <si>
+    <t>Arganda del Rey</t>
+  </si>
+  <si>
+    <t>El Atazar</t>
+  </si>
+  <si>
+    <t>Colmenar Viejo</t>
+  </si>
+  <si>
+    <t>Collado Villalba</t>
+  </si>
+  <si>
+    <t>Coslada</t>
+  </si>
+  <si>
+    <t>Fuenlabrada</t>
+  </si>
+  <si>
+    <t>Getafe</t>
+  </si>
+  <si>
+    <t>Guadalix de la Sierra</t>
+  </si>
+  <si>
+    <t>Leganés</t>
+  </si>
+  <si>
+    <t>Majadahonda</t>
+  </si>
+  <si>
+    <t>Móstoles</t>
+  </si>
+  <si>
+    <t>Orusco de Tajuña</t>
+  </si>
+  <si>
+    <t>Rascafría (Puerto de Cotos)</t>
+  </si>
+  <si>
+    <t>Rivas-Vaciamadrid</t>
+  </si>
+  <si>
+    <t>San Martín de Valdeiglesias</t>
+  </si>
+  <si>
+    <t>Torrejón de Ardoz</t>
+  </si>
+  <si>
+    <t>Valdemoro</t>
+  </si>
+  <si>
+    <t>Villa del Prado</t>
+  </si>
+  <si>
+    <t>Villarejo de Salvanés</t>
+  </si>
+  <si>
+    <t>Urbana</t>
+  </si>
+  <si>
+    <t>Suburbana</t>
+  </si>
+  <si>
+    <t>Rural</t>
+  </si>
+  <si>
+    <t>Urbana tráfico</t>
+  </si>
+  <si>
+    <t>Urbana fondo</t>
+  </si>
+  <si>
+    <t>Tráfico</t>
+  </si>
+  <si>
+    <t>Fondo</t>
+  </si>
+  <si>
+    <t>Industrial</t>
+  </si>
+  <si>
+    <t>estacion_tipo_area</t>
+  </si>
+  <si>
+    <t>estacion_tipo_estacion</t>
+  </si>
+  <si>
+    <t>C.E.I.P. Manuel Azaña, Avda. del Ejército, 5</t>
+  </si>
+  <si>
+    <t>Parque de Andalucía, C/ Pintor Murillo</t>
+  </si>
+  <si>
+    <t>Colegio Blas de Otero, Avda. del Oeste, 4</t>
+  </si>
+  <si>
+    <t>Parque Europa, C/ Humilladero con C/ Francisco Quevedo</t>
+  </si>
+  <si>
+    <t>Polideportivo Municipal Agustín Marañón, C/ Moreras (C/ Primero de Mayo, 4)</t>
+  </si>
+  <si>
+    <t>Punto Limpio, C/ Río Tajuña, 5</t>
+  </si>
+  <si>
+    <t>Instalaciones del Canal de Isabel II</t>
+  </si>
+  <si>
+    <t>Auditorio Municipal, C/ Molino de Viento, s/n</t>
+  </si>
+  <si>
+    <t>Colegio Público Rosa Chacel, C/ Santa Teresa de Jesús, 12</t>
+  </si>
+  <si>
+    <t>Polideportivo Municipal Valle Aguado, Avda. José Gárate, 8 (C/ Perú, 17)</t>
+  </si>
+  <si>
+    <t>C/ Grecia, 3 (trasera)</t>
+  </si>
+  <si>
+    <t>C.E.I.P. Mariana Pineda, Avda. de las Ciudades, 33</t>
+  </si>
+  <si>
+    <t>Camino de Chozas, s/n</t>
+  </si>
+  <si>
+    <t>C.E.P.A. Rosalía de Castro, C/ Roncal (Avda. de la Mancha, 50)</t>
+  </si>
+  <si>
+    <t>Campo de golf, C/ Isaac Albéniz</t>
+  </si>
+  <si>
+    <t>Parque Liana</t>
+  </si>
+  <si>
+    <t>Camino forestal de acceso al repetidor de telefonía</t>
+  </si>
+  <si>
+    <t>Centro de Visitantes Peñalara, Ctra. M-604, km 42 (Puerto de Cotos, Rascafría)</t>
+  </si>
+  <si>
+    <t>Polideportivo Cerro del Telégrafo, C/ Juncal (Avda. Los Almendros, 1)</t>
+  </si>
+  <si>
+    <t>C/ Depósito s/n</t>
+  </si>
+  <si>
+    <t>Parque del Ocio</t>
+  </si>
+  <si>
+    <t>Colegio Público Pedro Antonio de Alarcón, C/ Artemisa, 5</t>
+  </si>
+  <si>
+    <t>Hospital Virgen de la Poveda, C/ Alejandro Peris Barrios, km. 5</t>
+  </si>
+  <si>
+    <t>I.E.S. Nuestra Señora de la Victoria de Lepanto, C/ Luis de Requesens, 1-3</t>
   </si>
 </sst>
 </file>
@@ -826,7 +1139,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -836,7 +1149,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -862,7 +1174,6 @@
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
@@ -879,6 +1190,7 @@
     <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
@@ -939,7 +1251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -974,7 +1286,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1183,10 +1495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,11 +1507,9 @@
     <col min="2" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>48</v>
       </c>
@@ -1215,20 +1525,26 @@
       <c r="E1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="H1" s="10" t="s">
+      <c r="F1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>28079004</v>
       </c>
@@ -1244,20 +1560,23 @@
       <c r="E2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="9">
-        <v>-37122567</v>
-      </c>
-      <c r="G2" s="9">
-        <v>404238823</v>
-      </c>
-      <c r="H2">
+      <c r="F2">
         <v>-3.7121972222222199</v>
       </c>
-      <c r="I2">
+      <c r="G2">
         <v>40.423883333333301</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H2" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>28079008</v>
       </c>
@@ -1273,20 +1592,23 @@
       <c r="E3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="9">
-        <v>-36823158</v>
-      </c>
-      <c r="G3" s="9">
-        <v>404215533</v>
-      </c>
-      <c r="H3">
+      <c r="F3">
         <v>-3.6822833333333298</v>
       </c>
-      <c r="I3">
+      <c r="G3">
         <v>40.421563888888798</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>28079011</v>
       </c>
@@ -1302,20 +1624,23 @@
       <c r="E4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="9">
-        <v>-36773491</v>
-      </c>
-      <c r="G4" s="9">
-        <v>404514734</v>
-      </c>
-      <c r="H4">
+      <c r="F4">
         <v>-3.67736111111111</v>
       </c>
-      <c r="I4">
+      <c r="G4">
         <v>40.451469444444399</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>28079016</v>
       </c>
@@ -1331,20 +1656,23 @@
       <c r="E5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="9">
-        <v>-36392422</v>
-      </c>
-      <c r="G5" s="9">
-        <v>404400457</v>
-      </c>
-      <c r="H5">
+      <c r="F5">
         <v>-3.6392138888888801</v>
       </c>
-      <c r="I5">
+      <c r="G5">
         <v>40.440055555555503</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>28079017</v>
       </c>
@@ -1360,20 +1688,23 @@
       <c r="E6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="9">
-        <v>-37133167</v>
-      </c>
-      <c r="G6" s="9">
-        <v>40347147</v>
-      </c>
-      <c r="H6">
+      <c r="F6">
         <v>-3.7133027777777698</v>
       </c>
-      <c r="I6">
+      <c r="G6">
         <v>40.347149999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>28079018</v>
       </c>
@@ -1389,20 +1720,23 @@
       <c r="E7" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="9">
-        <v>-37318356</v>
-      </c>
-      <c r="G7" s="9">
-        <v>403947825</v>
-      </c>
-      <c r="H7">
+      <c r="F7">
         <v>-3.73183611111111</v>
       </c>
-      <c r="I7">
+      <c r="G7">
         <v>40.394783333333301</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>28079024</v>
       </c>
@@ -1418,20 +1752,23 @@
       <c r="E8" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F8" s="9">
-        <v>-37473445</v>
-      </c>
-      <c r="G8" s="9">
-        <v>404193577</v>
-      </c>
-      <c r="H8">
+      <c r="F8">
         <v>-3.7473444444444399</v>
       </c>
-      <c r="I8">
+      <c r="G8">
         <v>40.4193583333333</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>28079027</v>
       </c>
@@ -1447,20 +1784,23 @@
       <c r="E9" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="9">
-        <v>-35800258</v>
-      </c>
-      <c r="G9" s="9">
-        <v>404769179</v>
-      </c>
-      <c r="H9">
+      <c r="F9">
         <v>-3.58002777777777</v>
       </c>
-      <c r="I9">
+      <c r="G9">
         <v>40.476925000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>28079035</v>
       </c>
@@ -1476,20 +1816,23 @@
       <c r="E10" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="9">
-        <v>-37031662</v>
-      </c>
-      <c r="G10" s="9">
-        <v>404192091</v>
-      </c>
-      <c r="H10">
+      <c r="F10">
         <v>-3.7031666666666601</v>
       </c>
-      <c r="I10">
+      <c r="G10">
         <v>40.419208333333302</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>28079036</v>
       </c>
@@ -1505,20 +1848,23 @@
       <c r="E11" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="9">
-        <v>-36453104</v>
-      </c>
-      <c r="G11" s="9">
-        <v>404079517</v>
-      </c>
-      <c r="H11">
+      <c r="F11">
         <v>-3.6452833333333299</v>
       </c>
-      <c r="I11">
+      <c r="G11">
         <v>40.407955555555503</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>28079038</v>
       </c>
@@ -1534,20 +1880,23 @@
       <c r="E12" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="9">
-        <v>-37071303</v>
-      </c>
-      <c r="G12" s="9">
-        <v>404455439</v>
-      </c>
-      <c r="H12">
+      <c r="F12">
         <v>-3.7071222222222202</v>
       </c>
-      <c r="I12">
+      <c r="G12">
         <v>40.445547222222203</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>28079039</v>
       </c>
@@ -1563,20 +1912,23 @@
       <c r="E13" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="9">
-        <v>-37115364</v>
-      </c>
-      <c r="G13" s="9">
-        <v>404782322</v>
-      </c>
-      <c r="H13">
+      <c r="F13">
         <v>-3.7115361111111098</v>
       </c>
-      <c r="I13">
+      <c r="G13">
         <v>40.4782333333333</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>28079040</v>
       </c>
@@ -1592,20 +1944,23 @@
       <c r="E14" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="9">
-        <v>-36515286</v>
-      </c>
-      <c r="G14" s="9">
-        <v>403881478</v>
-      </c>
-      <c r="H14">
+      <c r="F14">
         <v>-3.6515277777777699</v>
       </c>
-      <c r="I14">
+      <c r="G14">
         <v>40.388147222222202</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>28079047</v>
       </c>
@@ -1621,20 +1976,23 @@
       <c r="E15" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="9">
-        <v>-36868138</v>
-      </c>
-      <c r="G15" s="9">
-        <v>403980991</v>
-      </c>
-      <c r="H15">
+      <c r="F15">
         <v>-3.6868249999999998</v>
       </c>
-      <c r="I15">
+      <c r="G15">
         <v>40.398102777777702</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>28079048</v>
       </c>
@@ -1650,20 +2008,23 @@
       <c r="E16" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F16" s="9">
-        <v>-36903729</v>
-      </c>
-      <c r="G16" s="9">
-        <v>404398904</v>
-      </c>
-      <c r="H16">
+      <c r="F16">
         <v>-3.6903722222222202</v>
       </c>
-      <c r="I16">
+      <c r="G16">
         <v>40.439891666666597</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>28079049</v>
       </c>
@@ -1674,25 +2035,28 @@
         <v>4473981.74</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="F17" s="9">
-        <v>-3.6824999999999904E+16</v>
-      </c>
-      <c r="G17" s="9">
-        <v>4041444444444440</v>
-      </c>
-      <c r="H17">
+        <v>100</v>
+      </c>
+      <c r="F17">
         <v>-3.6824999999999899</v>
       </c>
-      <c r="I17">
+      <c r="G17">
         <v>40.414444444444399</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H17" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>28079050</v>
       </c>
@@ -1708,20 +2072,23 @@
       <c r="E18" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="9">
-        <v>-36887449</v>
-      </c>
-      <c r="G18" s="9">
-        <v>404655841</v>
-      </c>
-      <c r="H18">
+      <c r="F18">
         <v>-3.6887444444444402</v>
       </c>
-      <c r="I18">
+      <c r="G18">
         <v>40.465583333333299</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>28079054</v>
       </c>
@@ -1737,20 +2104,23 @@
       <c r="E19" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F19" s="9">
-        <v>-36121394</v>
-      </c>
-      <c r="G19" s="9">
-        <v>403730118</v>
-      </c>
-      <c r="H19">
+      <c r="F19">
         <v>-3.6121388888888801</v>
       </c>
-      <c r="I19">
+      <c r="G19">
         <v>40.373011111111097</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>28079055</v>
       </c>
@@ -1766,20 +2136,23 @@
       <c r="E20" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="9">
-        <v>-35805649</v>
-      </c>
-      <c r="G20" s="9">
-        <v>404623628</v>
-      </c>
-      <c r="H20">
+      <c r="F20">
         <v>-3.58056388888888</v>
       </c>
-      <c r="I20">
+      <c r="G20">
         <v>40.462363888888802</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H20" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>28079056</v>
       </c>
@@ -1795,20 +2168,23 @@
       <c r="E21" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F21" s="9">
-        <v>-37187679</v>
-      </c>
-      <c r="G21" s="9">
-        <v>403850336</v>
-      </c>
-      <c r="H21">
+      <c r="F21">
         <v>-3.7187611111111099</v>
       </c>
-      <c r="I21">
+      <c r="G21">
         <v>40.385027777777701</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H21" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>28079057</v>
       </c>
@@ -1824,20 +2200,23 @@
       <c r="E22" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="9">
-        <v>-36605173</v>
-      </c>
-      <c r="G22" s="9">
-        <v>404942012</v>
-      </c>
-      <c r="H22">
+      <c r="F22">
         <v>-3.66051666666666</v>
       </c>
-      <c r="I22">
+      <c r="G22">
         <v>40.494199999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>28079058</v>
       </c>
@@ -1853,20 +2232,23 @@
       <c r="E23" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F23" s="9">
-        <v>-37746101</v>
-      </c>
-      <c r="G23" s="9">
-        <v>405180701</v>
-      </c>
-      <c r="H23">
+      <c r="F23">
         <v>-3.7746166666666601</v>
       </c>
-      <c r="I23">
+      <c r="G23">
         <v>40.518047222222201</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H23" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>28079059</v>
       </c>
@@ -1882,20 +2264,23 @@
       <c r="E24" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F24" s="9">
-        <v>-36163407</v>
-      </c>
-      <c r="G24" s="9">
-        <v>404607255</v>
-      </c>
-      <c r="H24">
+      <c r="F24">
         <v>-3.6091666666666602</v>
       </c>
-      <c r="I24">
+      <c r="G24">
         <v>40.4652777777777</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H24" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>28079060</v>
       </c>
@@ -1911,20 +2296,23 @@
       <c r="E25" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F25" s="9">
-        <v>-36897308</v>
-      </c>
-      <c r="G25" s="9">
-        <v>405005477</v>
-      </c>
-      <c r="H25">
+      <c r="F25">
         <v>-3.68973055555555</v>
       </c>
-      <c r="I25">
+      <c r="G25">
         <v>40.500547222222202</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H25" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>28005002</v>
       </c>
@@ -1940,14 +2328,26 @@
       <c r="E26" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H26">
+      <c r="F26">
         <v>-3.3777777777777702</v>
       </c>
-      <c r="I26">
+      <c r="G26">
         <v>40.4791666666666</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H26" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>28006004</v>
       </c>
@@ -1963,14 +2363,26 @@
       <c r="E27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H27">
+      <c r="F27">
         <v>-3.645</v>
       </c>
-      <c r="I27">
+      <c r="G27">
         <v>40.540277777777703</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H27" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>28007004</v>
       </c>
@@ -1986,14 +2398,26 @@
       <c r="E28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H28">
+      <c r="F28">
         <v>-3.83361111111111</v>
       </c>
-      <c r="I28">
+      <c r="G28">
         <v>40.341666666666598</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H28" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28009001</v>
       </c>
@@ -2009,14 +2433,26 @@
       <c r="E29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H29">
+      <c r="F29">
         <v>-3.5030555555555498</v>
       </c>
-      <c r="I29">
+      <c r="G29">
         <v>40.599722222222198</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H29" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28013002</v>
       </c>
@@ -2032,14 +2468,26 @@
       <c r="E30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H30">
+      <c r="F30">
         <v>-3.5913888888888801</v>
       </c>
-      <c r="I30">
+      <c r="G30">
         <v>40.033055555555499</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H30" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28014002</v>
       </c>
@@ -2055,14 +2503,26 @@
       <c r="E31" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H31">
+      <c r="F31">
         <v>-3.4588888888888798</v>
       </c>
-      <c r="I31">
+      <c r="G31">
         <v>40.300555555555498</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H31" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>28016001</v>
       </c>
@@ -2078,14 +2538,26 @@
       <c r="E32" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H32">
+      <c r="F32">
         <v>-3.4677777777777701</v>
       </c>
-      <c r="I32">
+      <c r="G32">
         <v>40.908888888888796</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H32" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>28045002</v>
       </c>
@@ -2101,14 +2573,26 @@
       <c r="E33" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H33">
+      <c r="F33">
         <v>-3.7738888888888802</v>
       </c>
-      <c r="I33">
+      <c r="G33">
         <v>40.664444444444399</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H33" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>28047002</v>
       </c>
@@ -2124,14 +2608,26 @@
       <c r="E34" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H34">
+      <c r="F34">
         <v>-4.01416666666666</v>
       </c>
-      <c r="I34">
+      <c r="G34">
         <v>40.633055555555501</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H34" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>28049003</v>
       </c>
@@ -2147,14 +2643,26 @@
       <c r="E35" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H35">
+      <c r="F35">
         <v>-3.5422222222222199</v>
       </c>
-      <c r="I35">
+      <c r="G35">
         <v>40.430277777777697</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H35" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>28058004</v>
       </c>
@@ -2170,14 +2678,26 @@
       <c r="E36" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H36">
+      <c r="F36">
         <v>-3.8008333333333302</v>
       </c>
-      <c r="I36">
+      <c r="G36">
         <v>40.281388888888799</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H36" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>28065014</v>
       </c>
@@ -2193,14 +2713,26 @@
       <c r="E37" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H37">
+      <c r="F37">
         <v>-3.7166666666666601</v>
       </c>
-      <c r="I37">
+      <c r="G37">
         <v>40.314444444444398</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H37" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="K37" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>28067001</v>
       </c>
@@ -2216,14 +2748,26 @@
       <c r="E38" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H38">
+      <c r="F38">
         <v>-3.70194444444444</v>
       </c>
-      <c r="I38">
+      <c r="G38">
         <v>40.780555555555502</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H38" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="J38" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="K38" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>28074007</v>
       </c>
@@ -2239,14 +2783,26 @@
       <c r="E39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H39">
+      <c r="F39">
         <v>-3.7544444444444398</v>
       </c>
-      <c r="I39">
+      <c r="G39">
         <v>40.3397222222222</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H39" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="J39" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="K39" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>28080003</v>
       </c>
@@ -2262,14 +2818,26 @@
       <c r="E40" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H40">
+      <c r="F40">
         <v>-3.8688888888888799</v>
       </c>
-      <c r="I40">
+      <c r="G40">
         <v>40.446111111111101</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H40" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>28092005</v>
       </c>
@@ -2285,14 +2853,26 @@
       <c r="E41" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H41">
+      <c r="F41">
         <v>-3.8766666666666598</v>
       </c>
-      <c r="I41">
+      <c r="G41">
         <v>40.324166666666599</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H41" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>28102001</v>
       </c>
@@ -2308,14 +2888,26 @@
       <c r="E42" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H42">
+      <c r="F42">
         <v>-3.2211111111111101</v>
       </c>
-      <c r="I42">
+      <c r="G42">
         <v>40.287500000000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H42" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="J42" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="K42" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>28120001</v>
       </c>
@@ -2331,14 +2923,26 @@
       <c r="E43" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H43">
+      <c r="F43">
         <v>-3.9611111111111099</v>
       </c>
-      <c r="I43">
+      <c r="G43">
         <v>40.825000000000003</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H43" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>28123002</v>
       </c>
@@ -2354,14 +2958,26 @@
       <c r="E44" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H44">
+      <c r="F44">
         <v>-3.5427777777777698</v>
       </c>
-      <c r="I44">
+      <c r="G44">
         <v>40.359722222222203</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H44" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="K44" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>28133002</v>
       </c>
@@ -2377,14 +2993,26 @@
       <c r="E45" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H45">
+      <c r="F45">
         <v>-4.3980555555555503</v>
       </c>
-      <c r="I45">
+      <c r="G45">
         <v>40.3675</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H45" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="K45" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>28148004</v>
       </c>
@@ -2400,14 +3028,26 @@
       <c r="E46" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H46">
+      <c r="F46">
         <v>-3.4775</v>
       </c>
-      <c r="I46">
+      <c r="G46">
         <v>40.449444444444403</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H46" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="J46" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="K46" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>28161001</v>
       </c>
@@ -2423,14 +3063,26 @@
       <c r="E47" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H47">
+      <c r="F47">
         <v>-3.68027777777777</v>
       </c>
-      <c r="I47">
+      <c r="G47">
         <v>40.184999999999903</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H47" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="K47" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>28171001</v>
       </c>
@@ -2446,14 +3098,26 @@
       <c r="E48" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H48">
+      <c r="F48">
         <v>-4.2755555555555498</v>
       </c>
-      <c r="I48">
+      <c r="G48">
         <v>40.248611111111103</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H48" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="K48" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>28180001</v>
       </c>
@@ -2469,11 +3133,23 @@
       <c r="E49" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H49">
+      <c r="F49">
         <v>-3.2766666666666602</v>
       </c>
-      <c r="I49">
+      <c r="G49">
         <v>40.1672222222222</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="J49" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="K49" s="7" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Nombre de estaciones en Coordenadas de estaciones y correción en doc"
This reverts commit aea0c1e275e7910434c8c035a996d663edd86997.
</commit_message>
<xml_diff>
--- a/Coordenadas_estaciones.xlsx
+++ b/Coordenadas_estaciones.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Compartido\Big Data\Github\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjuarez\Downloads\DatosSusana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C86D372-9D11-49E5-87AC-6920000B3080}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>03°22'40,0"W</t>
   </si>
@@ -337,159 +336,12 @@
   </si>
   <si>
     <t>Longitud</t>
-  </si>
-  <si>
-    <t>NOMBRE_ESTACION</t>
-  </si>
-  <si>
-    <t>PLAZA ESPAÑA</t>
-  </si>
-  <si>
-    <t>ESCUELAS AGUIRRE</t>
-  </si>
-  <si>
-    <t>AVDA. RAMÓN Y CAJAL</t>
-  </si>
-  <si>
-    <t>ARTURO SORIA</t>
-  </si>
-  <si>
-    <t>VILLAVERDE</t>
-  </si>
-  <si>
-    <t>FAROLILLO</t>
-  </si>
-  <si>
-    <t>CASA DE CAMPO</t>
-  </si>
-  <si>
-    <t>BARAJAS PUEBLO</t>
-  </si>
-  <si>
-    <t>PLAZA DEL CARMEN</t>
-  </si>
-  <si>
-    <t>MORATALAZ</t>
-  </si>
-  <si>
-    <t>CUATRO CAMINOS</t>
-  </si>
-  <si>
-    <t>BARRIO DEL PILAR</t>
-  </si>
-  <si>
-    <t>VALLECAS</t>
-  </si>
-  <si>
-    <t>MENDEZ ÁLVARO</t>
-  </si>
-  <si>
-    <t>CASTELLANA</t>
-  </si>
-  <si>
-    <t>PARQUE DEL RETIRO</t>
-  </si>
-  <si>
-    <t>PLAZA CASTILLA</t>
-  </si>
-  <si>
-    <t>ENSANCHE DE VALLECAS</t>
-  </si>
-  <si>
-    <t>URB. EMBAJADA</t>
-  </si>
-  <si>
-    <t>PLAZA ELÍPTICA</t>
-  </si>
-  <si>
-    <t>SANCHINARRO</t>
-  </si>
-  <si>
-    <t>EL PARDO</t>
-  </si>
-  <si>
-    <t>JUAN CARLOS I</t>
-  </si>
-  <si>
-    <t>TRES OLIVOS</t>
-  </si>
-  <si>
-    <t>ALCALÁ DE HENARES</t>
-  </si>
-  <si>
-    <t>ALCOBENDAS</t>
-  </si>
-  <si>
-    <t>ALCORCÓN</t>
-  </si>
-  <si>
-    <t>ALGETE</t>
-  </si>
-  <si>
-    <t>ARANJUEZ</t>
-  </si>
-  <si>
-    <t>ARGANDA DEL REY</t>
-  </si>
-  <si>
-    <t>EL ATAZAR</t>
-  </si>
-  <si>
-    <t>COLMENAR VIEJO</t>
-  </si>
-  <si>
-    <t>COLLADO VILLALBA</t>
-  </si>
-  <si>
-    <t>COSLADA</t>
-  </si>
-  <si>
-    <t>FUENLABRADA</t>
-  </si>
-  <si>
-    <t>GETAFE</t>
-  </si>
-  <si>
-    <t>GUADALIX DE LA SIERRA</t>
-  </si>
-  <si>
-    <t>LEGANÉS</t>
-  </si>
-  <si>
-    <t>MAJADAHONDA</t>
-  </si>
-  <si>
-    <t>MÓSTOLES</t>
-  </si>
-  <si>
-    <t>ORUSCO DE TAJUÑA</t>
-  </si>
-  <si>
-    <t>PUERTO DE COTOS</t>
-  </si>
-  <si>
-    <t>RIVAS-VACIAMADRID</t>
-  </si>
-  <si>
-    <t>SAN MARTÍN DE VALDEIGLESIAS</t>
-  </si>
-  <si>
-    <t>TORREJÓN DE ARDOZ</t>
-  </si>
-  <si>
-    <t>VALDEMORO</t>
-  </si>
-  <si>
-    <t>VILLA DEL PRADO</t>
-  </si>
-  <si>
-    <t>VILLAREJO DE SALVANÉS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1006,7 +858,7 @@
     <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
@@ -1120,23 +972,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1172,23 +1007,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1364,11 +1182,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,1431 +1195,1285 @@
     <col min="2" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>105</v>
+        <v>48</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="J1" s="10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>106</v>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>28079004</v>
       </c>
       <c r="B2" s="7">
-        <v>28079004</v>
+        <v>439579.32909999997</v>
       </c>
       <c r="C2" s="7">
-        <v>439579.32909999997</v>
-      </c>
-      <c r="D2" s="5">
         <v>4475049.2630000003</v>
       </c>
+      <c r="D2" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="E2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="9" t="s">
         <v>52</v>
       </c>
+      <c r="F2" s="9">
+        <v>-37122567</v>
+      </c>
       <c r="G2" s="9">
-        <v>-37122567</v>
-      </c>
-      <c r="H2" s="9">
         <v>404238823</v>
       </c>
+      <c r="H2">
+        <v>-3.7121972222222199</v>
+      </c>
       <c r="I2">
-        <v>-3.7121972219999999</v>
-      </c>
-      <c r="J2">
-        <v>40.423883330000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>107</v>
+        <v>40.423883333333301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>28079008</v>
       </c>
       <c r="B3" s="7">
-        <v>28079008</v>
+        <v>442117.2366</v>
       </c>
       <c r="C3" s="7">
-        <v>442117.2366</v>
-      </c>
-      <c r="D3" s="5">
         <v>4474770.6960000005</v>
       </c>
+      <c r="D3" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="E3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="9" t="s">
         <v>54</v>
       </c>
+      <c r="F3" s="9">
+        <v>-36823158</v>
+      </c>
       <c r="G3" s="9">
-        <v>-36823158</v>
-      </c>
-      <c r="H3" s="9">
         <v>404215533</v>
       </c>
+      <c r="H3">
+        <v>-3.6822833333333298</v>
+      </c>
       <c r="I3">
-        <v>-3.682283333</v>
-      </c>
-      <c r="J3">
-        <v>40.421563890000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>108</v>
+        <v>40.421563888888798</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>28079011</v>
       </c>
       <c r="B4" s="7">
-        <v>28079011</v>
+        <v>442564.04570000002</v>
       </c>
       <c r="C4" s="7">
-        <v>442564.04570000002</v>
-      </c>
-      <c r="D4" s="5">
         <v>4478088.5949999997</v>
       </c>
+      <c r="D4" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="E4" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="9" t="s">
         <v>56</v>
       </c>
+      <c r="F4" s="9">
+        <v>-36773491</v>
+      </c>
       <c r="G4" s="9">
-        <v>-36773491</v>
-      </c>
-      <c r="H4" s="9">
         <v>404514734</v>
       </c>
+      <c r="H4">
+        <v>-3.67736111111111</v>
+      </c>
       <c r="I4">
-        <v>-3.6773611110000002</v>
-      </c>
-      <c r="J4">
-        <v>40.451469439999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>109</v>
+        <v>40.451469444444399</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>28079016</v>
       </c>
       <c r="B5" s="7">
-        <v>28079016</v>
+        <v>445786.17290000001</v>
       </c>
       <c r="C5" s="7">
-        <v>445786.17290000001</v>
-      </c>
-      <c r="D5" s="5">
         <v>4476796.0190000003</v>
       </c>
+      <c r="D5" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="E5" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" s="9" t="s">
         <v>58</v>
       </c>
+      <c r="F5" s="9">
+        <v>-36392422</v>
+      </c>
       <c r="G5" s="9">
-        <v>-36392422</v>
-      </c>
-      <c r="H5" s="9">
         <v>404400457</v>
       </c>
+      <c r="H5">
+        <v>-3.6392138888888801</v>
+      </c>
       <c r="I5">
-        <v>-3.6392138890000001</v>
-      </c>
-      <c r="J5">
-        <v>40.440055559999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>110</v>
+        <v>40.440055555555503</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>28079017</v>
       </c>
       <c r="B6" s="7">
-        <v>28079017</v>
+        <v>439420.70150000002</v>
       </c>
       <c r="C6" s="7">
-        <v>439420.70150000002</v>
-      </c>
-      <c r="D6" s="5">
         <v>4466532.4550000001</v>
       </c>
+      <c r="D6" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E6" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="9" t="s">
         <v>60</v>
       </c>
+      <c r="F6" s="9">
+        <v>-37133167</v>
+      </c>
       <c r="G6" s="9">
-        <v>-37133167</v>
-      </c>
-      <c r="H6" s="9">
         <v>40347147</v>
       </c>
+      <c r="H6">
+        <v>-3.7133027777777698</v>
+      </c>
       <c r="I6">
-        <v>-3.7133027780000001</v>
-      </c>
-      <c r="J6">
         <v>40.347149999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>111</v>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>28079018</v>
       </c>
       <c r="B7" s="7">
-        <v>28079018</v>
+        <v>437891.6961</v>
       </c>
       <c r="C7" s="7">
-        <v>437891.6961</v>
-      </c>
-      <c r="D7" s="5">
         <v>4471832.7690000003</v>
       </c>
+      <c r="D7" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="E7" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="9" t="s">
         <v>62</v>
       </c>
+      <c r="F7" s="9">
+        <v>-37318356</v>
+      </c>
       <c r="G7" s="9">
-        <v>-37318356</v>
-      </c>
-      <c r="H7" s="9">
         <v>403947825</v>
       </c>
+      <c r="H7">
+        <v>-3.73183611111111</v>
+      </c>
       <c r="I7">
-        <v>-3.7318361109999998</v>
-      </c>
-      <c r="J7">
-        <v>40.394783330000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>112</v>
+        <v>40.394783333333301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>28079024</v>
       </c>
       <c r="B8" s="7">
-        <v>28079024</v>
+        <v>436598.5637</v>
       </c>
       <c r="C8" s="7">
-        <v>436598.5637</v>
-      </c>
-      <c r="D8" s="5">
         <v>4474571.6179999998</v>
       </c>
+      <c r="D8" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="E8" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="9" t="s">
         <v>64</v>
       </c>
+      <c r="F8" s="9">
+        <v>-37473445</v>
+      </c>
       <c r="G8" s="9">
-        <v>-37473445</v>
-      </c>
-      <c r="H8" s="9">
         <v>404193577</v>
       </c>
+      <c r="H8">
+        <v>-3.7473444444444399</v>
+      </c>
       <c r="I8">
-        <v>-3.7473444439999999</v>
-      </c>
-      <c r="J8">
-        <v>40.419358330000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>113</v>
+        <v>40.4193583333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>28079027</v>
       </c>
       <c r="B9" s="7">
-        <v>28079027</v>
+        <v>450835.20260000002</v>
       </c>
       <c r="C9" s="7">
-        <v>450835.20260000002</v>
-      </c>
-      <c r="D9" s="5">
         <v>4480854.1720000003</v>
       </c>
+      <c r="D9" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="E9" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="9" t="s">
         <v>66</v>
       </c>
+      <c r="F9" s="9">
+        <v>-35800258</v>
+      </c>
       <c r="G9" s="9">
-        <v>-35800258</v>
-      </c>
-      <c r="H9" s="9">
         <v>404769179</v>
       </c>
+      <c r="H9">
+        <v>-3.58002777777777</v>
+      </c>
       <c r="I9">
-        <v>-3.5800277779999998</v>
-      </c>
-      <c r="J9">
         <v>40.476925000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>114</v>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>28079035</v>
       </c>
       <c r="B10" s="7">
-        <v>28079035</v>
+        <v>440346.36190000002</v>
       </c>
       <c r="C10" s="7">
-        <v>440346.36190000002</v>
-      </c>
-      <c r="D10" s="5">
         <v>4474524.3569999998</v>
       </c>
+      <c r="D10" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="E10" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" s="9" t="s">
         <v>68</v>
       </c>
+      <c r="F10" s="9">
+        <v>-37031662</v>
+      </c>
       <c r="G10" s="9">
-        <v>-37031662</v>
-      </c>
-      <c r="H10" s="9">
         <v>404192091</v>
       </c>
+      <c r="H10">
+        <v>-3.7031666666666601</v>
+      </c>
       <c r="I10">
-        <v>-3.7031666670000001</v>
-      </c>
-      <c r="J10">
-        <v>40.419208329999996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>115</v>
+        <v>40.419208333333302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>28079036</v>
       </c>
       <c r="B11" s="7">
-        <v>28079036</v>
+        <v>445245.51299999998</v>
       </c>
       <c r="C11" s="7">
-        <v>445245.51299999998</v>
-      </c>
-      <c r="D11" s="5">
         <v>4473237.3490000004</v>
       </c>
+      <c r="D11" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="E11" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="9" t="s">
         <v>70</v>
       </c>
+      <c r="F11" s="9">
+        <v>-36453104</v>
+      </c>
       <c r="G11" s="9">
-        <v>-36453104</v>
-      </c>
-      <c r="H11" s="9">
         <v>404079517</v>
       </c>
+      <c r="H11">
+        <v>-3.6452833333333299</v>
+      </c>
       <c r="I11">
-        <v>-3.6452833330000001</v>
-      </c>
-      <c r="J11">
-        <v>40.407955559999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>116</v>
+        <v>40.407955555555503</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>28079038</v>
       </c>
       <c r="B12" s="7">
-        <v>28079038</v>
+        <v>440033.4632</v>
       </c>
       <c r="C12" s="7">
-        <v>440033.4632</v>
-      </c>
-      <c r="D12" s="5">
         <v>4477450.2110000001</v>
       </c>
+      <c r="D12" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="E12" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="9" t="s">
         <v>72</v>
       </c>
+      <c r="F12" s="9">
+        <v>-37071303</v>
+      </c>
       <c r="G12" s="9">
-        <v>-37071303</v>
-      </c>
-      <c r="H12" s="9">
         <v>404455439</v>
       </c>
+      <c r="H12">
+        <v>-3.7071222222222202</v>
+      </c>
       <c r="I12">
-        <v>-3.7071222220000002</v>
-      </c>
-      <c r="J12">
-        <v>40.445547220000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>117</v>
+        <v>40.445547222222203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>28079039</v>
       </c>
       <c r="B13" s="7">
-        <v>28079039</v>
+        <v>439689.04960000003</v>
       </c>
       <c r="C13" s="7">
-        <v>439689.04960000003</v>
-      </c>
-      <c r="D13" s="5">
         <v>4481081.6189999999</v>
       </c>
+      <c r="D13" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="E13" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="9" t="s">
         <v>74</v>
       </c>
+      <c r="F13" s="9">
+        <v>-37115364</v>
+      </c>
       <c r="G13" s="9">
-        <v>-37115364</v>
-      </c>
-      <c r="H13" s="9">
         <v>404782322</v>
       </c>
+      <c r="H13">
+        <v>-3.7115361111111098</v>
+      </c>
       <c r="I13">
-        <v>-3.711536111</v>
-      </c>
-      <c r="J13">
-        <v>40.478233330000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>118</v>
+        <v>40.4782333333333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>28079040</v>
       </c>
       <c r="B14" s="7">
-        <v>28079040</v>
+        <v>444701.68709999998</v>
       </c>
       <c r="C14" s="7">
-        <v>444701.68709999998</v>
-      </c>
-      <c r="D14" s="5">
         <v>4471043.01</v>
       </c>
+      <c r="D14" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="E14" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="9" t="s">
         <v>76</v>
       </c>
+      <c r="F14" s="9">
+        <v>-36515286</v>
+      </c>
       <c r="G14" s="9">
-        <v>-36515286</v>
-      </c>
-      <c r="H14" s="9">
         <v>403881478</v>
       </c>
+      <c r="H14">
+        <v>-3.6515277777777699</v>
+      </c>
       <c r="I14">
-        <v>-3.6515277780000002</v>
-      </c>
-      <c r="J14">
-        <v>40.38814722</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>119</v>
+        <v>40.388147222222202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>28079047</v>
       </c>
       <c r="B15" s="7">
-        <v>28079047</v>
+        <v>441715.43030000001</v>
       </c>
       <c r="C15" s="7">
-        <v>441715.43030000001</v>
-      </c>
-      <c r="D15" s="5">
         <v>4472170.2489999998</v>
       </c>
+      <c r="D15" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="E15" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15" s="9" t="s">
         <v>78</v>
       </c>
+      <c r="F15" s="9">
+        <v>-36868138</v>
+      </c>
       <c r="G15" s="9">
-        <v>-36868138</v>
-      </c>
-      <c r="H15" s="9">
         <v>403980991</v>
       </c>
+      <c r="H15">
+        <v>-3.6868249999999998</v>
+      </c>
       <c r="I15">
-        <v>-3.6868249999999998</v>
-      </c>
-      <c r="J15">
-        <v>40.398102780000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>120</v>
+        <v>40.398102777777702</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>28079048</v>
       </c>
       <c r="B16" s="7">
-        <v>28079048</v>
+        <v>441449.63410000002</v>
       </c>
       <c r="C16" s="7">
-        <v>441449.63410000002</v>
-      </c>
-      <c r="D16" s="5">
         <v>4476811.42</v>
       </c>
+      <c r="D16" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="E16" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="9" t="s">
         <v>80</v>
       </c>
+      <c r="F16" s="9">
+        <v>-36903729</v>
+      </c>
       <c r="G16" s="9">
-        <v>-36903729</v>
-      </c>
-      <c r="H16" s="9">
         <v>404398904</v>
       </c>
+      <c r="H16">
+        <v>-3.6903722222222202</v>
+      </c>
       <c r="I16">
-        <v>-3.6903722220000001</v>
-      </c>
-      <c r="J16">
-        <v>40.439891670000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>121</v>
+        <v>40.439891666666597</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>28079049</v>
       </c>
       <c r="B17" s="7">
-        <v>28079049</v>
+        <v>442095.52</v>
       </c>
       <c r="C17" s="7">
-        <v>442095.52</v>
-      </c>
-      <c r="D17" s="5">
         <v>4473981.74</v>
       </c>
+      <c r="D17" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="E17" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F17" s="9" t="s">
         <v>102</v>
       </c>
+      <c r="F17" s="9">
+        <v>-3.6824999999999904E+16</v>
+      </c>
       <c r="G17" s="9">
-        <v>-3.6824999999999904E+16</v>
-      </c>
-      <c r="H17" s="9">
         <v>4041444444444440</v>
       </c>
+      <c r="H17">
+        <v>-3.6824999999999899</v>
+      </c>
       <c r="I17">
-        <v>-3.6825000000000001</v>
-      </c>
-      <c r="J17">
-        <v>40.414444439999997</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>122</v>
+        <v>40.414444444444399</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>28079050</v>
       </c>
       <c r="B18" s="7">
-        <v>28079050</v>
+        <v>441609.9474</v>
       </c>
       <c r="C18" s="7">
-        <v>441609.9474</v>
-      </c>
-      <c r="D18" s="5">
         <v>4479662.3459999999</v>
       </c>
+      <c r="D18" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="E18" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" s="9" t="s">
         <v>82</v>
       </c>
+      <c r="F18" s="9">
+        <v>-36887449</v>
+      </c>
       <c r="G18" s="9">
-        <v>-36887449</v>
-      </c>
-      <c r="H18" s="9">
         <v>404655841</v>
       </c>
+      <c r="H18">
+        <v>-3.6887444444444402</v>
+      </c>
       <c r="I18">
-        <v>-3.6887444440000001</v>
-      </c>
-      <c r="J18">
-        <v>40.465583330000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>123</v>
+        <v>40.465583333333299</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>28079054</v>
       </c>
       <c r="B19" s="7">
-        <v>28079054</v>
+        <v>448033.22629999998</v>
       </c>
       <c r="C19" s="7">
-        <v>448033.22629999998</v>
-      </c>
-      <c r="D19" s="5">
         <v>4469339.0439999998</v>
       </c>
+      <c r="D19" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="E19" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F19" s="9" t="s">
         <v>84</v>
       </c>
+      <c r="F19" s="9">
+        <v>-36121394</v>
+      </c>
       <c r="G19" s="9">
-        <v>-36121394</v>
-      </c>
-      <c r="H19" s="9">
         <v>403730118</v>
       </c>
+      <c r="H19">
+        <v>-3.6121388888888801</v>
+      </c>
       <c r="I19">
-        <v>-3.6121388890000001</v>
-      </c>
-      <c r="J19">
-        <v>40.37301111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>124</v>
+        <v>40.373011111111097</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>28079055</v>
       </c>
       <c r="B20" s="7">
-        <v>28079055</v>
+        <v>450778.88390000002</v>
       </c>
       <c r="C20" s="7">
-        <v>450778.88390000002</v>
-      </c>
-      <c r="D20" s="5">
         <v>4479238.8629999999</v>
       </c>
+      <c r="D20" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="E20" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F20" s="9" t="s">
         <v>86</v>
       </c>
+      <c r="F20" s="9">
+        <v>-35805649</v>
+      </c>
       <c r="G20" s="9">
-        <v>-35805649</v>
-      </c>
-      <c r="H20" s="9">
         <v>404623628</v>
       </c>
+      <c r="H20">
+        <v>-3.58056388888888</v>
+      </c>
       <c r="I20">
-        <v>-3.580563889</v>
-      </c>
-      <c r="J20">
-        <v>40.462363889999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>125</v>
+        <v>40.462363888888802</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>28079056</v>
       </c>
       <c r="B21" s="7">
-        <v>28079056</v>
+        <v>438991.91609999997</v>
       </c>
       <c r="C21" s="7">
-        <v>438991.91609999997</v>
-      </c>
-      <c r="D21" s="5">
         <v>4470741.5480000004</v>
       </c>
+      <c r="D21" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="E21" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F21" s="9" t="s">
         <v>88</v>
       </c>
+      <c r="F21" s="9">
+        <v>-37187679</v>
+      </c>
       <c r="G21" s="9">
-        <v>-37187679</v>
-      </c>
-      <c r="H21" s="9">
         <v>403850336</v>
       </c>
+      <c r="H21">
+        <v>-3.7187611111111099</v>
+      </c>
       <c r="I21">
-        <v>-3.7187611110000001</v>
-      </c>
-      <c r="J21">
-        <v>40.385027780000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>126</v>
+        <v>40.385027777777701</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>28079057</v>
       </c>
       <c r="B22" s="7">
-        <v>28079057</v>
+        <v>444026.80800000002</v>
       </c>
       <c r="C22" s="7">
-        <v>444026.80800000002</v>
-      </c>
-      <c r="D22" s="5">
         <v>4482820.5810000002</v>
       </c>
+      <c r="D22" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="E22" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F22" s="9" t="s">
         <v>90</v>
       </c>
+      <c r="F22" s="9">
+        <v>-36605173</v>
+      </c>
       <c r="G22" s="9">
-        <v>-36605173</v>
-      </c>
-      <c r="H22" s="9">
         <v>404942012</v>
       </c>
+      <c r="H22">
+        <v>-3.66051666666666</v>
+      </c>
       <c r="I22">
-        <v>-3.660516667</v>
-      </c>
-      <c r="J22">
         <v>40.494199999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>127</v>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>28079058</v>
       </c>
       <c r="B23" s="7">
-        <v>28079058</v>
+        <v>434381.6</v>
       </c>
       <c r="C23" s="7">
-        <v>434381.6</v>
-      </c>
-      <c r="D23" s="5">
         <v>4485548.7</v>
       </c>
+      <c r="D23" s="5" t="s">
+        <v>91</v>
+      </c>
       <c r="E23" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F23" s="9" t="s">
         <v>92</v>
       </c>
+      <c r="F23" s="9">
+        <v>-37746101</v>
+      </c>
       <c r="G23" s="9">
-        <v>-37746101</v>
-      </c>
-      <c r="H23" s="9">
         <v>405180701</v>
       </c>
+      <c r="H23">
+        <v>-3.7746166666666601</v>
+      </c>
       <c r="I23">
-        <v>-3.7746166670000001</v>
-      </c>
-      <c r="J23">
-        <v>40.51804722</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>128</v>
+        <v>40.518047222222201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>28079059</v>
       </c>
       <c r="B24" s="7">
-        <v>28079059</v>
+        <v>447744.46659999999</v>
       </c>
       <c r="C24" s="7">
-        <v>447744.46659999999</v>
-      </c>
-      <c r="D24" s="5">
         <v>4479077.6780000003</v>
       </c>
+      <c r="D24" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="E24" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F24" s="9" t="s">
         <v>94</v>
       </c>
+      <c r="F24" s="9">
+        <v>-36163407</v>
+      </c>
       <c r="G24" s="9">
-        <v>-36163407</v>
-      </c>
-      <c r="H24" s="9">
         <v>404607255</v>
       </c>
+      <c r="H24">
+        <v>-3.6091666666666602</v>
+      </c>
       <c r="I24">
-        <v>-3.6091666670000002</v>
-      </c>
-      <c r="J24">
-        <v>40.465277780000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>129</v>
+        <v>40.4652777777777</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>28079060</v>
       </c>
       <c r="B25" s="7">
-        <v>28079060</v>
+        <v>441556.70049999998</v>
       </c>
       <c r="C25" s="7">
-        <v>441556.70049999998</v>
-      </c>
-      <c r="D25" s="5">
         <v>4483543.9939999999</v>
       </c>
+      <c r="D25" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="E25" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F25" s="9" t="s">
         <v>96</v>
       </c>
+      <c r="F25" s="9">
+        <v>-36897308</v>
+      </c>
       <c r="G25" s="9">
-        <v>-36897308</v>
-      </c>
-      <c r="H25" s="9">
         <v>405005477</v>
       </c>
+      <c r="H25">
+        <v>-3.68973055555555</v>
+      </c>
       <c r="I25">
-        <v>-3.6897305560000002</v>
-      </c>
-      <c r="J25">
-        <v>40.500547220000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>130</v>
+        <v>40.500547222222202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>28005002</v>
       </c>
       <c r="B26" s="2">
-        <v>28005002</v>
+        <v>467979</v>
       </c>
       <c r="C26" s="2">
-        <v>467979</v>
-      </c>
-      <c r="D26" s="2">
         <v>4481011</v>
       </c>
+      <c r="D26" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="E26" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F26" t="s">
         <v>1</v>
       </c>
+      <c r="H26">
+        <v>-3.3777777777777702</v>
+      </c>
       <c r="I26">
-        <v>-3.377777778</v>
-      </c>
-      <c r="J26">
-        <v>40.479166669999998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>131</v>
+        <v>40.4791666666666</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>28006004</v>
       </c>
       <c r="B27" s="2">
-        <v>28006004</v>
+        <v>445363</v>
       </c>
       <c r="C27" s="2">
-        <v>445363</v>
-      </c>
-      <c r="D27" s="2">
         <v>4487950</v>
       </c>
+      <c r="D27" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="E27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F27" t="s">
         <v>3</v>
       </c>
+      <c r="H27">
+        <v>-3.645</v>
+      </c>
       <c r="I27">
-        <v>-3.645</v>
-      </c>
-      <c r="J27">
-        <v>40.540277779999997</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>132</v>
+        <v>40.540277777777703</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>28007004</v>
       </c>
       <c r="B28" s="2">
-        <v>28007004</v>
+        <v>429190</v>
       </c>
       <c r="C28" s="2">
-        <v>429190</v>
-      </c>
-      <c r="D28" s="2">
         <v>4466041</v>
       </c>
+      <c r="D28" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F28" t="s">
         <v>5</v>
       </c>
+      <c r="H28">
+        <v>-3.83361111111111</v>
+      </c>
       <c r="I28">
-        <v>-3.8336111110000002</v>
-      </c>
-      <c r="J28">
-        <v>40.341666670000002</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>133</v>
+        <v>40.341666666666598</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28009001</v>
       </c>
       <c r="B29" s="2">
-        <v>28009001</v>
+        <v>457418</v>
       </c>
       <c r="C29" s="2">
-        <v>457418</v>
-      </c>
-      <c r="D29" s="2">
         <v>4494449</v>
       </c>
+      <c r="D29" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" t="s">
         <v>7</v>
       </c>
+      <c r="H29">
+        <v>-3.5030555555555498</v>
+      </c>
       <c r="I29">
-        <v>-3.5030555560000001</v>
-      </c>
-      <c r="J29">
-        <v>40.599722219999997</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>134</v>
+        <v>40.599722222222198</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>28013002</v>
       </c>
       <c r="B30" s="2">
-        <v>28013002</v>
+        <v>449541</v>
       </c>
       <c r="C30" s="2">
-        <v>449541</v>
-      </c>
-      <c r="D30" s="2">
         <v>4431618</v>
       </c>
+      <c r="D30" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E30" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F30" t="s">
         <v>9</v>
       </c>
+      <c r="H30">
+        <v>-3.5913888888888801</v>
+      </c>
       <c r="I30">
-        <v>-3.5913888890000001</v>
-      </c>
-      <c r="J30">
-        <v>40.033055560000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>135</v>
+        <v>40.033055555555499</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>28014002</v>
       </c>
       <c r="B31" s="2">
-        <v>28014002</v>
+        <v>461002</v>
       </c>
       <c r="C31" s="2">
-        <v>461002</v>
-      </c>
-      <c r="D31" s="2">
         <v>4461246</v>
       </c>
+      <c r="D31" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E31" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" t="s">
         <v>11</v>
       </c>
+      <c r="H31">
+        <v>-3.4588888888888798</v>
+      </c>
       <c r="I31">
-        <v>-3.4588888889999998</v>
-      </c>
-      <c r="J31">
-        <v>40.300555559999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>136</v>
+        <v>40.300555555555498</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>28016001</v>
       </c>
       <c r="B32" s="2">
-        <v>28016001</v>
+        <v>460596</v>
       </c>
       <c r="C32" s="2">
-        <v>460596</v>
-      </c>
-      <c r="D32" s="2">
         <v>4528767</v>
       </c>
+      <c r="D32" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" t="s">
         <v>13</v>
       </c>
+      <c r="H32">
+        <v>-3.4677777777777701</v>
+      </c>
       <c r="I32">
-        <v>-3.4677777779999999</v>
-      </c>
-      <c r="J32">
-        <v>40.90888889</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>137</v>
+        <v>40.908888888888796</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>28045002</v>
       </c>
       <c r="B33" s="2">
-        <v>28045002</v>
+        <v>434586</v>
       </c>
       <c r="C33" s="2">
-        <v>434586</v>
-      </c>
-      <c r="D33" s="2">
         <v>4501818</v>
       </c>
+      <c r="D33" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="E33" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" t="s">
         <v>15</v>
       </c>
+      <c r="H33">
+        <v>-3.7738888888888802</v>
+      </c>
       <c r="I33">
-        <v>-3.7738888890000002</v>
-      </c>
-      <c r="J33">
-        <v>40.664444439999997</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>138</v>
+        <v>40.664444444444399</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>28047002</v>
       </c>
       <c r="B34" s="2">
-        <v>28047002</v>
+        <v>414233</v>
       </c>
       <c r="C34" s="2">
-        <v>414233</v>
-      </c>
-      <c r="D34" s="2">
         <v>4498525</v>
       </c>
+      <c r="D34" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="E34" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" t="s">
         <v>17</v>
       </c>
+      <c r="H34">
+        <v>-4.01416666666666</v>
+      </c>
       <c r="I34">
-        <v>-4.0141666669999996</v>
-      </c>
-      <c r="J34">
-        <v>40.633055560000003</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>139</v>
+        <v>40.633055555555501</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>28049003</v>
       </c>
       <c r="B35" s="2">
-        <v>28049003</v>
+        <v>454001</v>
       </c>
       <c r="C35" s="2">
-        <v>454001</v>
-      </c>
-      <c r="D35" s="2">
         <v>4475678</v>
       </c>
+      <c r="D35" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E35" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F35" t="s">
         <v>19</v>
       </c>
+      <c r="H35">
+        <v>-3.5422222222222199</v>
+      </c>
       <c r="I35">
-        <v>-3.5422222219999999</v>
-      </c>
-      <c r="J35">
-        <v>40.430277779999997</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>140</v>
+        <v>40.430277777777697</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>28058004</v>
       </c>
       <c r="B36" s="2">
-        <v>28058004</v>
+        <v>431913</v>
       </c>
       <c r="C36" s="2">
-        <v>431913</v>
-      </c>
-      <c r="D36" s="2">
         <v>4459313</v>
       </c>
+      <c r="D36" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E36" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" t="s">
         <v>21</v>
       </c>
+      <c r="H36">
+        <v>-3.8008333333333302</v>
+      </c>
       <c r="I36">
-        <v>-3.8008333329999999</v>
-      </c>
-      <c r="J36">
-        <v>40.281388890000002</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>141</v>
+        <v>40.281388888888799</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>28065014</v>
       </c>
       <c r="B37" s="2">
-        <v>28065014</v>
+        <v>439090</v>
       </c>
       <c r="C37" s="2">
-        <v>439090</v>
-      </c>
-      <c r="D37" s="2">
         <v>4462920</v>
       </c>
+      <c r="D37" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E37" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F37" t="s">
         <v>23</v>
       </c>
+      <c r="H37">
+        <v>-3.7166666666666601</v>
+      </c>
       <c r="I37">
-        <v>-3.7166666670000001</v>
-      </c>
-      <c r="J37">
-        <v>40.314444440000003</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>142</v>
+        <v>40.314444444444398</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>28067001</v>
       </c>
       <c r="B38" s="2">
-        <v>28067001</v>
+        <v>440751</v>
       </c>
       <c r="C38" s="2">
-        <v>440751</v>
-      </c>
-      <c r="D38" s="2">
         <v>4514644</v>
       </c>
+      <c r="D38" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E38" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F38" t="s">
         <v>25</v>
       </c>
+      <c r="H38">
+        <v>-3.70194444444444</v>
+      </c>
       <c r="I38">
-        <v>-3.701944444</v>
-      </c>
-      <c r="J38">
-        <v>40.780555560000003</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>143</v>
+        <v>40.780555555555502</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>28074007</v>
       </c>
       <c r="B39" s="2">
-        <v>28074007</v>
+        <v>435914</v>
       </c>
       <c r="C39" s="2">
-        <v>435914</v>
-      </c>
-      <c r="D39" s="2">
         <v>4465744</v>
       </c>
+      <c r="D39" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E39" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F39" t="s">
         <v>27</v>
       </c>
+      <c r="H39">
+        <v>-3.7544444444444398</v>
+      </c>
       <c r="I39">
-        <v>-3.7544444440000002</v>
-      </c>
-      <c r="J39">
-        <v>40.339722219999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>144</v>
+        <v>40.3397222222222</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>28080003</v>
       </c>
       <c r="B40" s="2">
-        <v>28080003</v>
+        <v>426307</v>
       </c>
       <c r="C40" s="2">
-        <v>426307</v>
-      </c>
-      <c r="D40" s="2">
         <v>4477645</v>
       </c>
+      <c r="D40" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E40" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F40" t="s">
         <v>29</v>
       </c>
+      <c r="H40">
+        <v>-3.8688888888888799</v>
+      </c>
       <c r="I40">
-        <v>-3.8688888889999999</v>
-      </c>
-      <c r="J40">
-        <v>40.446111109999997</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>145</v>
+        <v>40.446111111111101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>28092005</v>
       </c>
       <c r="B41" s="2">
-        <v>28092005</v>
+        <v>425516</v>
       </c>
       <c r="C41" s="2">
-        <v>425516</v>
-      </c>
-      <c r="D41" s="2">
         <v>4464113</v>
       </c>
+      <c r="D41" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F41" t="s">
         <v>31</v>
       </c>
+      <c r="H41">
+        <v>-3.8766666666666598</v>
+      </c>
       <c r="I41">
-        <v>-3.8766666669999998</v>
-      </c>
-      <c r="J41">
-        <v>40.324166669999997</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>146</v>
+        <v>40.324166666666599</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>28102001</v>
       </c>
       <c r="B42" s="2">
-        <v>28102001</v>
+        <v>481205</v>
       </c>
       <c r="C42" s="2">
-        <v>481205</v>
-      </c>
-      <c r="D42" s="2">
         <v>4459700</v>
       </c>
+      <c r="D42" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F42" t="s">
         <v>33</v>
       </c>
+      <c r="H42">
+        <v>-3.2211111111111101</v>
+      </c>
       <c r="I42">
-        <v>-3.2211111109999999</v>
-      </c>
-      <c r="J42">
         <v>40.287500000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>147</v>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>28120001</v>
       </c>
       <c r="B43" s="2">
-        <v>28120001</v>
+        <v>418948</v>
       </c>
       <c r="C43" s="2">
-        <v>418948</v>
-      </c>
-      <c r="D43" s="2">
         <v>4519788</v>
       </c>
+      <c r="D43" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E43" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F43" t="s">
         <v>35</v>
       </c>
+      <c r="H43">
+        <v>-3.9611111111111099</v>
+      </c>
       <c r="I43">
-        <v>-3.9611111110000001</v>
-      </c>
-      <c r="J43">
         <v>40.825000000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>148</v>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>28123002</v>
       </c>
       <c r="B44" s="2">
-        <v>28123002</v>
+        <v>453906</v>
       </c>
       <c r="C44" s="2">
-        <v>453906</v>
-      </c>
-      <c r="D44" s="2">
         <v>4467829</v>
       </c>
+      <c r="D44" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="E44" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F44" t="s">
         <v>37</v>
       </c>
+      <c r="H44">
+        <v>-3.5427777777777698</v>
+      </c>
       <c r="I44">
-        <v>-3.542777778</v>
-      </c>
-      <c r="J44">
-        <v>40.359722220000002</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>149</v>
+        <v>40.359722222222203</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>28133002</v>
       </c>
       <c r="B45" s="2">
-        <v>28133002</v>
+        <v>381298</v>
       </c>
       <c r="C45" s="2">
-        <v>381298</v>
-      </c>
-      <c r="D45" s="2">
         <v>4469513</v>
       </c>
+      <c r="D45" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E45" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F45" t="s">
         <v>39</v>
       </c>
+      <c r="H45">
+        <v>-4.3980555555555503</v>
+      </c>
       <c r="I45">
-        <v>-4.3980555560000001</v>
-      </c>
-      <c r="J45">
         <v>40.3675</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>150</v>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>28148004</v>
       </c>
       <c r="B46" s="2">
-        <v>28148004</v>
+        <v>459497</v>
       </c>
       <c r="C46" s="2">
-        <v>459497</v>
-      </c>
-      <c r="D46" s="2">
         <v>4477765</v>
       </c>
+      <c r="D46" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="E46" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F46" t="s">
         <v>41</v>
       </c>
+      <c r="H46">
+        <v>-3.4775</v>
+      </c>
       <c r="I46">
-        <v>-3.4775</v>
-      </c>
-      <c r="J46">
-        <v>40.449444440000001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>151</v>
+        <v>40.449444444444403</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>28161001</v>
       </c>
       <c r="B47" s="2">
-        <v>28161001</v>
+        <v>442089</v>
       </c>
       <c r="C47" s="2">
-        <v>442089</v>
-      </c>
-      <c r="D47" s="2">
         <v>4448540</v>
       </c>
+      <c r="D47" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="E47" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F47" t="s">
         <v>43</v>
       </c>
+      <c r="H47">
+        <v>-3.68027777777777</v>
+      </c>
       <c r="I47">
-        <v>-3.6802777780000002</v>
-      </c>
-      <c r="J47">
-        <v>40.185000000000002</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>152</v>
+        <v>40.184999999999903</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>28171001</v>
       </c>
       <c r="B48" s="2">
-        <v>28171001</v>
+        <v>391504</v>
       </c>
       <c r="C48" s="2">
-        <v>391504</v>
-      </c>
-      <c r="D48" s="2">
         <v>4456144</v>
       </c>
+      <c r="D48" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="E48" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F48" t="s">
         <v>45</v>
       </c>
+      <c r="H48">
+        <v>-4.2755555555555498</v>
+      </c>
       <c r="I48">
-        <v>-4.2755555559999996</v>
-      </c>
-      <c r="J48">
-        <v>40.248611109999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>153</v>
+        <v>40.248611111111103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>28180001</v>
       </c>
       <c r="B49" s="2">
-        <v>28180001</v>
+        <v>476442</v>
       </c>
       <c r="C49" s="2">
-        <v>476442</v>
-      </c>
-      <c r="D49" s="2">
         <v>4446354</v>
       </c>
+      <c r="D49" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="E49" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F49" t="s">
         <v>47</v>
       </c>
+      <c r="H49">
+        <v>-3.2766666666666602</v>
+      </c>
       <c r="I49">
-        <v>-3.2766666670000002</v>
-      </c>
-      <c r="J49">
-        <v>40.167222219999999</v>
+        <v>40.1672222222222</v>
       </c>
     </row>
   </sheetData>
@@ -2810,7 +2482,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2822,7 +2494,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>